<commit_message>
Atualização automática de FORO_REGIONAL_DA_RESTINGA.xlsx
</commit_message>
<xml_diff>
--- a/FORO_REGIONAL_DA_RESTINGA.xlsx
+++ b/FORO_REGIONAL_DA_RESTINGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5FFBE9C-8589-4926-ABB4-182698812E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{263F6A28-180F-4FA3-AB9D-7D311FF5F0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1143,7 +1143,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{6C9FF19B-D0B6-46EC-AEE0-E95443236413}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{DFA3B634-2EAC-49B3-BE4E-220D97C49ABC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1173,10 +1173,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9909108C-5F0D-4116-A4E4-1C2B92D0AB5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D25D258-57B3-4A04-9F09-1E5A6ADCFBB2}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1214,7 +1214,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E59D184-8C69-4AFE-885C-0FD0120332BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{270FEB7A-6EE0-4C66-9D48-C39BE6FE812C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1277,7 +1277,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AF17CDC-C7B1-4590-B865-DE2D037A1D62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C81B4964-F448-4FCA-8B39-C46DBA620F50}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1296,7 +1296,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE0358A1-CEE8-ECFB-C457-2F7F391E6DB4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DD1F0D2-1AC1-25A4-A11A-CAF43979BC33}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1345,7 +1345,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{523EAC76-E565-A2E9-E404-EA2416A6A00F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEB83B73-4FCD-A198-CF2B-A5D911F6EEAA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1364,7 +1364,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6CE211-6A03-2A50-44E1-91506E325F72}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C69F8E6D-4F20-439D-F078-5CE358BBDA81}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1395,7 +1395,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B5DD2C-C7F6-4642-AF83-D14E9EEE8C51}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F930585-224E-B2BE-BCB1-2D7B245A58FD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1426,7 +1426,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C452EAE-359B-F97C-B23B-001D7961AE17}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A828CE8-4253-9E5E-DE62-0F8E606E150B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1469,7 +1469,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18EE518D-F3ED-441E-861C-F692EEE9F407}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAEA52AB-4315-40D9-872E-41067DFFB3C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1507,7 +1507,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B665E12E-0DCF-4B15-A8CD-2F9D835363C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4652FFC4-99E5-49F9-900A-0D84717C0C0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1550,7 +1550,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5574707-3B74-43E9-8065-FE649D9B55C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{791BA8D3-3A79-451D-BE38-895413594C90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1863,7 +1863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0886623E-036E-43DD-B9D3-0F15A21E855F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED306213-71C1-4B43-8A67-BAA3D6B7A0F9}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5313,16 +5313,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>